<commit_message>
Significant improvements to simulation.
</commit_message>
<xml_diff>
--- a/myDocs/Optimization Comparison.xlsx
+++ b/myDocs/Optimization Comparison.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\wgu\C950\myDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E41C096-CD5A-457D-B703-F9ABFB2437BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{946B26CD-8951-4094-93F4-7B124F8D40DC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="3" xr2:uid="{34BB5D8C-162D-47FA-95AA-753C2FC3244F}"/>
+    <workbookView xWindow="38280" yWindow="2775" windowWidth="29040" windowHeight="15840" xr2:uid="{34BB5D8C-162D-47FA-95AA-753C2FC3244F}"/>
   </bookViews>
   <sheets>
     <sheet name="BFS" sheetId="1" r:id="rId1"/>
@@ -669,8 +669,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50BA8E80-91ED-41F9-B71B-9957CFC8959D}">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2773,8 +2773,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BC5C9AF-FC5F-4139-BD83-91D8E4F2E409}">
   <dimension ref="A1:V43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Delivery deadlines being missed, improved interface to help identify. About to rework load_builder.
</commit_message>
<xml_diff>
--- a/myDocs/Optimization Comparison.xlsx
+++ b/myDocs/Optimization Comparison.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\wgu\C950\myDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{946B26CD-8951-4094-93F4-7B124F8D40DC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{399CBCB1-239A-406D-AAF8-613C32DD3CB3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="2775" windowWidth="29040" windowHeight="15840" xr2:uid="{34BB5D8C-162D-47FA-95AA-753C2FC3244F}"/>
+    <workbookView xWindow="39525" yWindow="4020" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{34BB5D8C-162D-47FA-95AA-753C2FC3244F}"/>
   </bookViews>
   <sheets>
     <sheet name="BFS" sheetId="1" r:id="rId1"/>
@@ -149,6 +149,7 @@
     </r>
     <r>
       <rPr>
+        <b/>
         <vertAlign val="superscript"/>
         <sz val="11"/>
         <color theme="1"/>
@@ -160,6 +161,7 @@
     </r>
     <r>
       <rPr>
+        <b/>
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
@@ -258,7 +260,7 @@
     <numFmt numFmtId="175" formatCode="#,###.00&quot;ms&quot;"/>
     <numFmt numFmtId="176" formatCode="0.0"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -275,14 +277,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <vertAlign val="superscript"/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -307,12 +301,21 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -321,16 +324,13 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -351,6 +351,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -669,8 +675,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50BA8E80-91ED-41F9-B71B-9957CFC8959D}">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G12" sqref="A1:G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -684,25 +690,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="3" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="16" t="s">
         <v>13</v>
       </c>
     </row>
@@ -722,11 +728,11 @@
       <c r="E2" s="1">
         <v>1.2E-2</v>
       </c>
-      <c r="F2" s="6">
+      <c r="F2" s="5">
         <f>FACT(B2)</f>
         <v>1</v>
       </c>
-      <c r="G2" s="7">
+      <c r="G2" s="6">
         <f>E2/F2*1000</f>
         <v>12</v>
       </c>
@@ -747,11 +753,11 @@
       <c r="E3" s="1">
         <v>1.2999999999999999E-2</v>
       </c>
-      <c r="F3" s="6">
+      <c r="F3" s="5">
         <f t="shared" ref="F3:F12" si="0">FACT(B3)</f>
         <v>1</v>
       </c>
-      <c r="G3" s="7">
+      <c r="G3" s="6">
         <f t="shared" ref="G3:G12" si="1">E3/F3*1000</f>
         <v>13</v>
       </c>
@@ -772,11 +778,11 @@
       <c r="E4" s="1">
         <v>3.6999999999999998E-2</v>
       </c>
-      <c r="F4" s="6">
+      <c r="F4" s="5">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="G4" s="7">
+      <c r="G4" s="6">
         <f t="shared" si="1"/>
         <v>18.5</v>
       </c>
@@ -797,11 +803,11 @@
       <c r="E5" s="1">
         <v>0.14399999999999999</v>
       </c>
-      <c r="F5" s="6">
+      <c r="F5" s="5">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="G5" s="7">
+      <c r="G5" s="6">
         <f t="shared" si="1"/>
         <v>23.999999999999996</v>
       </c>
@@ -822,11 +828,11 @@
       <c r="E6" s="1">
         <v>0.73499999999999999</v>
       </c>
-      <c r="F6" s="6">
+      <c r="F6" s="5">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="G6" s="7">
+      <c r="G6" s="6">
         <f t="shared" si="1"/>
         <v>30.625</v>
       </c>
@@ -847,11 +853,11 @@
       <c r="E7" s="1">
         <v>4.1360000000000001</v>
       </c>
-      <c r="F7" s="6">
+      <c r="F7" s="5">
         <f t="shared" si="0"/>
         <v>120</v>
       </c>
-      <c r="G7" s="7">
+      <c r="G7" s="6">
         <f t="shared" si="1"/>
         <v>34.466666666666669</v>
       </c>
@@ -872,11 +878,11 @@
       <c r="E8" s="1">
         <v>27.68</v>
       </c>
-      <c r="F8" s="6">
+      <c r="F8" s="5">
         <f t="shared" si="0"/>
         <v>720</v>
       </c>
-      <c r="G8" s="7">
+      <c r="G8" s="6">
         <f t="shared" si="1"/>
         <v>38.444444444444443</v>
       </c>
@@ -897,11 +903,11 @@
       <c r="E9" s="1">
         <v>217.155</v>
       </c>
-      <c r="F9" s="6">
+      <c r="F9" s="5">
         <f t="shared" si="0"/>
         <v>5040</v>
       </c>
-      <c r="G9" s="7">
+      <c r="G9" s="6">
         <f t="shared" si="1"/>
         <v>43.086309523809526</v>
       </c>
@@ -922,11 +928,11 @@
       <c r="E10" s="1">
         <v>1939.7049999999999</v>
       </c>
-      <c r="F10" s="6">
+      <c r="F10" s="5">
         <f t="shared" si="0"/>
         <v>40320</v>
       </c>
-      <c r="G10" s="7">
+      <c r="G10" s="6">
         <f t="shared" si="1"/>
         <v>48.107762896825399</v>
       </c>
@@ -947,11 +953,11 @@
       <c r="E11" s="1">
         <v>19409.473000000002</v>
       </c>
-      <c r="F11" s="6">
+      <c r="F11" s="5">
         <f t="shared" si="0"/>
         <v>362880</v>
       </c>
-      <c r="G11" s="7">
+      <c r="G11" s="6">
         <f t="shared" si="1"/>
         <v>53.487304343033514</v>
       </c>
@@ -972,11 +978,11 @@
       <c r="E12" s="1">
         <v>213931.87100000001</v>
       </c>
-      <c r="F12" s="6">
+      <c r="F12" s="5">
         <f t="shared" si="0"/>
         <v>3628800</v>
       </c>
-      <c r="G12" s="7">
+      <c r="G12" s="6">
         <f t="shared" si="1"/>
         <v>58.953888613315698</v>
       </c>
@@ -991,8 +997,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D8A18A7-E53F-417D-A285-FCFBF4240C06}">
   <dimension ref="A1:G48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H40" sqref="H40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1004,25 +1010,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="3" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="12" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1033,7 +1039,7 @@
       <c r="B2" s="2">
         <v>0</v>
       </c>
-      <c r="C2" s="12">
+      <c r="C2" s="11">
         <v>0</v>
       </c>
       <c r="D2" t="s">
@@ -1042,11 +1048,11 @@
       <c r="E2" s="1">
         <v>2E-3</v>
       </c>
-      <c r="F2" s="6">
+      <c r="F2" s="5">
         <f>B2^2</f>
         <v>0</v>
       </c>
-      <c r="G2" s="8"/>
+      <c r="G2" s="7"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -1055,7 +1061,7 @@
       <c r="B3" s="2">
         <v>1</v>
       </c>
-      <c r="C3" s="12">
+      <c r="C3" s="11">
         <v>14.4</v>
       </c>
       <c r="D3" t="s">
@@ -1064,11 +1070,11 @@
       <c r="E3" s="1">
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="F3" s="6">
+      <c r="F3" s="5">
         <f>B3^3</f>
         <v>1</v>
       </c>
-      <c r="G3" s="5">
+      <c r="G3" s="4">
         <f>E3/F3*1000</f>
         <v>9</v>
       </c>
@@ -1080,7 +1086,7 @@
       <c r="B4" s="2">
         <v>2</v>
       </c>
-      <c r="C4" s="12">
+      <c r="C4" s="11">
         <v>18.100000000000001</v>
       </c>
       <c r="D4" t="s">
@@ -1089,11 +1095,11 @@
       <c r="E4" s="1">
         <v>1.6E-2</v>
       </c>
-      <c r="F4" s="6">
+      <c r="F4" s="5">
         <f t="shared" ref="F4:F48" si="0">B4^3</f>
         <v>8</v>
       </c>
-      <c r="G4" s="5">
+      <c r="G4" s="4">
         <f t="shared" ref="G4:G48" si="1">E4/F4*1000</f>
         <v>2</v>
       </c>
@@ -1105,7 +1111,7 @@
       <c r="B5" s="2">
         <v>3</v>
       </c>
-      <c r="C5" s="12">
+      <c r="C5" s="11">
         <v>28.3</v>
       </c>
       <c r="D5" t="s">
@@ -1114,11 +1120,11 @@
       <c r="E5" s="1">
         <v>3.3000000000000002E-2</v>
       </c>
-      <c r="F5" s="6">
+      <c r="F5" s="5">
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
-      <c r="G5" s="5">
+      <c r="G5" s="4">
         <f t="shared" si="1"/>
         <v>1.2222222222222221</v>
       </c>
@@ -1130,7 +1136,7 @@
       <c r="B6" s="2">
         <v>4</v>
       </c>
-      <c r="C6" s="12">
+      <c r="C6" s="11">
         <v>31.1</v>
       </c>
       <c r="D6" t="s">
@@ -1139,11 +1145,11 @@
       <c r="E6" s="1">
         <v>5.8999999999999997E-2</v>
       </c>
-      <c r="F6" s="6">
+      <c r="F6" s="5">
         <f t="shared" si="0"/>
         <v>64</v>
       </c>
-      <c r="G6" s="5">
+      <c r="G6" s="4">
         <f t="shared" si="1"/>
         <v>0.921875</v>
       </c>
@@ -1155,7 +1161,7 @@
       <c r="B7" s="2">
         <v>5</v>
       </c>
-      <c r="C7" s="12">
+      <c r="C7" s="11">
         <v>31.4</v>
       </c>
       <c r="D7" t="s">
@@ -1164,11 +1170,11 @@
       <c r="E7" s="1">
         <v>0.1</v>
       </c>
-      <c r="F7" s="6">
+      <c r="F7" s="5">
         <f t="shared" si="0"/>
         <v>125</v>
       </c>
-      <c r="G7" s="5">
+      <c r="G7" s="4">
         <f t="shared" si="1"/>
         <v>0.8</v>
       </c>
@@ -1180,7 +1186,7 @@
       <c r="B8" s="2">
         <v>6</v>
       </c>
-      <c r="C8" s="12">
+      <c r="C8" s="11">
         <v>35</v>
       </c>
       <c r="D8" t="s">
@@ -1189,11 +1195,11 @@
       <c r="E8" s="1">
         <v>0.16500000000000001</v>
       </c>
-      <c r="F8" s="6">
+      <c r="F8" s="5">
         <f t="shared" si="0"/>
         <v>216</v>
       </c>
-      <c r="G8" s="5">
+      <c r="G8" s="4">
         <f t="shared" si="1"/>
         <v>0.76388888888888895</v>
       </c>
@@ -1205,7 +1211,7 @@
       <c r="B9" s="2">
         <v>7</v>
       </c>
-      <c r="C9" s="12">
+      <c r="C9" s="11">
         <v>35.4</v>
       </c>
       <c r="D9" t="s">
@@ -1214,11 +1220,11 @@
       <c r="E9" s="1">
         <v>0.251</v>
       </c>
-      <c r="F9" s="6">
+      <c r="F9" s="5">
         <f t="shared" si="0"/>
         <v>343</v>
       </c>
-      <c r="G9" s="5">
+      <c r="G9" s="4">
         <f t="shared" si="1"/>
         <v>0.73177842565597673</v>
       </c>
@@ -1230,7 +1236,7 @@
       <c r="B10" s="2">
         <v>8</v>
       </c>
-      <c r="C10" s="12">
+      <c r="C10" s="11">
         <v>35.799999999999997</v>
       </c>
       <c r="D10" t="s">
@@ -1239,11 +1245,11 @@
       <c r="E10" s="1">
         <v>0.35799999999999998</v>
       </c>
-      <c r="F10" s="6">
+      <c r="F10" s="5">
         <f t="shared" si="0"/>
         <v>512</v>
       </c>
-      <c r="G10" s="5">
+      <c r="G10" s="4">
         <f t="shared" si="1"/>
         <v>0.69921875</v>
       </c>
@@ -1255,7 +1261,7 @@
       <c r="B11" s="2">
         <v>9</v>
       </c>
-      <c r="C11" s="12">
+      <c r="C11" s="11">
         <v>36.1</v>
       </c>
       <c r="D11" t="s">
@@ -1264,11 +1270,11 @@
       <c r="E11" s="1">
         <v>0.497</v>
       </c>
-      <c r="F11" s="6">
+      <c r="F11" s="5">
         <f t="shared" si="0"/>
         <v>729</v>
       </c>
-      <c r="G11" s="5">
+      <c r="G11" s="4">
         <f t="shared" si="1"/>
         <v>0.68175582990397809</v>
       </c>
@@ -1280,7 +1286,7 @@
       <c r="B12" s="2">
         <v>10</v>
       </c>
-      <c r="C12" s="12">
+      <c r="C12" s="11">
         <v>32.5</v>
       </c>
       <c r="D12" t="s">
@@ -1289,11 +1295,11 @@
       <c r="E12" s="1">
         <v>0.72399999999999998</v>
       </c>
-      <c r="F12" s="6">
+      <c r="F12" s="5">
         <f t="shared" si="0"/>
         <v>1000</v>
       </c>
-      <c r="G12" s="5">
+      <c r="G12" s="4">
         <f t="shared" si="1"/>
         <v>0.72399999999999998</v>
       </c>
@@ -1305,7 +1311,7 @@
       <c r="B13" s="2">
         <v>11</v>
       </c>
-      <c r="C13" s="12">
+      <c r="C13" s="11">
         <v>32.9</v>
       </c>
       <c r="D13" t="s">
@@ -1314,11 +1320,11 @@
       <c r="E13" s="1">
         <v>0.878</v>
       </c>
-      <c r="F13" s="6">
+      <c r="F13" s="5">
         <f t="shared" si="0"/>
         <v>1331</v>
       </c>
-      <c r="G13" s="5">
+      <c r="G13" s="4">
         <f t="shared" si="1"/>
         <v>0.65965439519158531</v>
       </c>
@@ -1330,7 +1336,7 @@
       <c r="B14" s="2">
         <v>12</v>
       </c>
-      <c r="C14" s="12">
+      <c r="C14" s="11">
         <v>33.5</v>
       </c>
       <c r="D14" t="s">
@@ -1339,11 +1345,11 @@
       <c r="E14" s="1">
         <v>1.2</v>
       </c>
-      <c r="F14" s="6">
+      <c r="F14" s="5">
         <f t="shared" si="0"/>
         <v>1728</v>
       </c>
-      <c r="G14" s="5">
+      <c r="G14" s="4">
         <f t="shared" si="1"/>
         <v>0.69444444444444442</v>
       </c>
@@ -1355,7 +1361,7 @@
       <c r="B15" s="2">
         <v>13</v>
       </c>
-      <c r="C15" s="12">
+      <c r="C15" s="11">
         <v>35</v>
       </c>
       <c r="D15" t="s">
@@ -1364,11 +1370,11 @@
       <c r="E15" s="1">
         <v>1.421</v>
       </c>
-      <c r="F15" s="6">
+      <c r="F15" s="5">
         <f t="shared" si="0"/>
         <v>2197</v>
       </c>
-      <c r="G15" s="5">
+      <c r="G15" s="4">
         <f t="shared" si="1"/>
         <v>0.64679107874374153</v>
       </c>
@@ -1380,7 +1386,7 @@
       <c r="B16" s="2">
         <v>14</v>
       </c>
-      <c r="C16" s="12">
+      <c r="C16" s="11">
         <v>36.700000000000003</v>
       </c>
       <c r="D16" t="s">
@@ -1389,11 +1395,11 @@
       <c r="E16" s="1">
         <v>1.774</v>
       </c>
-      <c r="F16" s="6">
+      <c r="F16" s="5">
         <f t="shared" si="0"/>
         <v>2744</v>
       </c>
-      <c r="G16" s="5">
+      <c r="G16" s="4">
         <f t="shared" si="1"/>
         <v>0.64650145772594747</v>
       </c>
@@ -1405,7 +1411,7 @@
       <c r="B17" s="2">
         <v>15</v>
       </c>
-      <c r="C17" s="12">
+      <c r="C17" s="11">
         <v>37.4</v>
       </c>
       <c r="D17" t="s">
@@ -1414,11 +1420,11 @@
       <c r="E17" s="1">
         <v>2.1800000000000002</v>
       </c>
-      <c r="F17" s="6">
+      <c r="F17" s="5">
         <f t="shared" si="0"/>
         <v>3375</v>
       </c>
-      <c r="G17" s="5">
+      <c r="G17" s="4">
         <f t="shared" si="1"/>
         <v>0.64592592592592601</v>
       </c>
@@ -1430,7 +1436,7 @@
       <c r="B18" s="2">
         <v>16</v>
       </c>
-      <c r="C18" s="12">
+      <c r="C18" s="11">
         <v>43.5</v>
       </c>
       <c r="D18" t="s">
@@ -1439,11 +1445,11 @@
       <c r="E18" s="1">
         <v>2.4409999999999998</v>
       </c>
-      <c r="F18" s="6">
+      <c r="F18" s="5">
         <f t="shared" si="0"/>
         <v>4096</v>
       </c>
-      <c r="G18" s="5">
+      <c r="G18" s="4">
         <f t="shared" si="1"/>
         <v>0.595947265625</v>
       </c>
@@ -1455,7 +1461,7 @@
       <c r="B19" s="2">
         <v>17</v>
       </c>
-      <c r="C19" s="12">
+      <c r="C19" s="11">
         <v>43.8</v>
       </c>
       <c r="D19" t="s">
@@ -1464,11 +1470,11 @@
       <c r="E19" s="1">
         <v>2.867</v>
       </c>
-      <c r="F19" s="6">
+      <c r="F19" s="5">
         <f t="shared" si="0"/>
         <v>4913</v>
       </c>
-      <c r="G19" s="5">
+      <c r="G19" s="4">
         <f t="shared" si="1"/>
         <v>0.58355383675961736</v>
       </c>
@@ -1480,7 +1486,7 @@
       <c r="B20" s="2">
         <v>18</v>
       </c>
-      <c r="C20" s="12">
+      <c r="C20" s="11">
         <v>48.1</v>
       </c>
       <c r="D20" t="s">
@@ -1489,11 +1495,11 @@
       <c r="E20" s="1">
         <v>3.4129999999999998</v>
       </c>
-      <c r="F20" s="6">
+      <c r="F20" s="5">
         <f t="shared" si="0"/>
         <v>5832</v>
       </c>
-      <c r="G20" s="5">
+      <c r="G20" s="4">
         <f t="shared" si="1"/>
         <v>0.58521947873799729</v>
       </c>
@@ -1505,7 +1511,7 @@
       <c r="B21" s="2">
         <v>19</v>
       </c>
-      <c r="C21" s="12">
+      <c r="C21" s="11">
         <v>42.6</v>
       </c>
       <c r="D21" t="s">
@@ -1514,11 +1520,11 @@
       <c r="E21" s="1">
         <v>4.0060000000000002</v>
       </c>
-      <c r="F21" s="6">
+      <c r="F21" s="5">
         <f t="shared" si="0"/>
         <v>6859</v>
       </c>
-      <c r="G21" s="5">
+      <c r="G21" s="4">
         <f t="shared" si="1"/>
         <v>0.58405015308353991</v>
       </c>
@@ -1530,7 +1536,7 @@
       <c r="B22" s="2">
         <v>20</v>
       </c>
-      <c r="C22" s="12">
+      <c r="C22" s="11">
         <v>48.4</v>
       </c>
       <c r="D22" t="s">
@@ -1539,11 +1545,11 @@
       <c r="E22" s="1">
         <v>4.8360000000000003</v>
       </c>
-      <c r="F22" s="6">
+      <c r="F22" s="5">
         <f t="shared" si="0"/>
         <v>8000</v>
       </c>
-      <c r="G22" s="5">
+      <c r="G22" s="4">
         <f t="shared" si="1"/>
         <v>0.60450000000000004</v>
       </c>
@@ -1555,7 +1561,7 @@
       <c r="B23" s="2">
         <v>21</v>
       </c>
-      <c r="C23" s="12">
+      <c r="C23" s="11">
         <v>52.1</v>
       </c>
       <c r="D23" t="s">
@@ -1564,11 +1570,11 @@
       <c r="E23" s="1">
         <v>5.4530000000000003</v>
       </c>
-      <c r="F23" s="6">
+      <c r="F23" s="5">
         <f t="shared" si="0"/>
         <v>9261</v>
       </c>
-      <c r="G23" s="5">
+      <c r="G23" s="4">
         <f t="shared" si="1"/>
         <v>0.58881330309901747</v>
       </c>
@@ -1580,7 +1586,7 @@
       <c r="B24" s="2">
         <v>22</v>
       </c>
-      <c r="C24" s="12">
+      <c r="C24" s="11">
         <v>52.1</v>
       </c>
       <c r="D24" t="s">
@@ -1589,11 +1595,11 @@
       <c r="E24" s="1">
         <v>6.1029999999999998</v>
       </c>
-      <c r="F24" s="6">
+      <c r="F24" s="5">
         <f t="shared" si="0"/>
         <v>10648</v>
       </c>
-      <c r="G24" s="5">
+      <c r="G24" s="4">
         <f t="shared" si="1"/>
         <v>0.57315927873779116</v>
       </c>
@@ -1605,7 +1611,7 @@
       <c r="B25" s="2">
         <v>23</v>
       </c>
-      <c r="C25" s="12">
+      <c r="C25" s="11">
         <v>51.2</v>
       </c>
       <c r="D25" t="s">
@@ -1614,11 +1620,11 @@
       <c r="E25" s="1">
         <v>6.9210000000000003</v>
       </c>
-      <c r="F25" s="6">
+      <c r="F25" s="5">
         <f t="shared" si="0"/>
         <v>12167</v>
       </c>
-      <c r="G25" s="5">
+      <c r="G25" s="4">
         <f t="shared" si="1"/>
         <v>0.5688337305827238</v>
       </c>
@@ -1630,7 +1636,7 @@
       <c r="B26" s="2">
         <v>24</v>
       </c>
-      <c r="C26" s="12">
+      <c r="C26" s="11">
         <v>51.9</v>
       </c>
       <c r="D26" t="s">
@@ -1639,11 +1645,11 @@
       <c r="E26" s="1">
         <v>8.3539999999999992</v>
       </c>
-      <c r="F26" s="6">
+      <c r="F26" s="5">
         <f t="shared" si="0"/>
         <v>13824</v>
       </c>
-      <c r="G26" s="5">
+      <c r="G26" s="4">
         <f t="shared" si="1"/>
         <v>0.60431134259259245</v>
       </c>
@@ -1655,7 +1661,7 @@
       <c r="B27" s="2">
         <v>25</v>
       </c>
-      <c r="C27" s="12">
+      <c r="C27" s="11">
         <v>52.2</v>
       </c>
       <c r="D27" t="s">
@@ -1664,11 +1670,11 @@
       <c r="E27" s="1">
         <v>8.9359999999999999</v>
       </c>
-      <c r="F27" s="6">
+      <c r="F27" s="5">
         <f t="shared" si="0"/>
         <v>15625</v>
       </c>
-      <c r="G27" s="5">
+      <c r="G27" s="4">
         <f t="shared" si="1"/>
         <v>0.57190400000000008</v>
       </c>
@@ -1680,20 +1686,20 @@
       <c r="B28" s="2">
         <v>24</v>
       </c>
-      <c r="C28" s="12">
+      <c r="C28" s="11">
         <v>51.9</v>
       </c>
       <c r="D28" t="s">
         <v>21</v>
       </c>
-      <c r="E28" s="9">
+      <c r="E28" s="8">
         <v>7.9969999999999999</v>
       </c>
-      <c r="F28" s="6">
+      <c r="F28" s="5">
         <f t="shared" si="0"/>
         <v>13824</v>
       </c>
-      <c r="G28" s="5">
+      <c r="G28" s="4">
         <f t="shared" si="1"/>
         <v>0.57848668981481477</v>
       </c>
@@ -1705,20 +1711,20 @@
       <c r="B29" s="2">
         <v>49</v>
       </c>
-      <c r="C29" s="12">
+      <c r="C29" s="11">
         <v>56.85</v>
       </c>
       <c r="D29" t="s">
         <v>26</v>
       </c>
-      <c r="E29" s="9">
+      <c r="E29" s="8">
         <v>69.635000000000005</v>
       </c>
-      <c r="F29" s="6">
+      <c r="F29" s="5">
         <f t="shared" si="0"/>
         <v>117649</v>
       </c>
-      <c r="G29" s="5">
+      <c r="G29" s="4">
         <f t="shared" si="1"/>
         <v>0.59188773385239146</v>
       </c>
@@ -1730,20 +1736,20 @@
       <c r="B30" s="2">
         <v>74</v>
       </c>
-      <c r="C30" s="12">
+      <c r="C30" s="11">
         <v>61.62</v>
       </c>
       <c r="D30" t="s">
         <v>25</v>
       </c>
-      <c r="E30" s="9">
+      <c r="E30" s="8">
         <v>242.64599999999999</v>
       </c>
-      <c r="F30" s="6">
+      <c r="F30" s="5">
         <f t="shared" si="0"/>
         <v>405224</v>
       </c>
-      <c r="G30" s="5">
+      <c r="G30" s="4">
         <f t="shared" si="1"/>
         <v>0.59879474068663252</v>
       </c>
@@ -1755,20 +1761,20 @@
       <c r="B31" s="2">
         <v>99</v>
       </c>
-      <c r="C31" s="12">
+      <c r="C31" s="11">
         <v>51.69</v>
       </c>
       <c r="D31" t="s">
         <v>21</v>
       </c>
-      <c r="E31" s="9">
+      <c r="E31" s="8">
         <v>580.61199999999997</v>
       </c>
-      <c r="F31" s="6">
+      <c r="F31" s="5">
         <f t="shared" si="0"/>
         <v>970299</v>
       </c>
-      <c r="G31" s="5">
+      <c r="G31" s="4">
         <f t="shared" si="1"/>
         <v>0.5983846216475539</v>
       </c>
@@ -1780,20 +1786,20 @@
       <c r="B32" s="2">
         <v>124</v>
       </c>
-      <c r="C32" s="12">
+      <c r="C32" s="11">
         <v>57.43</v>
       </c>
       <c r="D32" t="s">
         <v>26</v>
       </c>
-      <c r="E32" s="9">
+      <c r="E32" s="8">
         <v>1083.5719999999999</v>
       </c>
-      <c r="F32" s="6">
+      <c r="F32" s="5">
         <f t="shared" si="0"/>
         <v>1906624</v>
       </c>
-      <c r="G32" s="5">
+      <c r="G32" s="4">
         <f t="shared" si="1"/>
         <v>0.56831971065086762</v>
       </c>
@@ -1805,20 +1811,20 @@
       <c r="B33" s="2">
         <v>149</v>
       </c>
-      <c r="C33" s="12">
+      <c r="C33" s="11">
         <v>55.74</v>
       </c>
       <c r="D33" t="s">
         <v>28</v>
       </c>
-      <c r="E33" s="9">
+      <c r="E33" s="8">
         <v>1952.914</v>
       </c>
-      <c r="F33" s="6">
+      <c r="F33" s="5">
         <f t="shared" si="0"/>
         <v>3307949</v>
       </c>
-      <c r="G33" s="5">
+      <c r="G33" s="4">
         <f t="shared" si="1"/>
         <v>0.59037004500371681</v>
       </c>
@@ -1830,20 +1836,20 @@
       <c r="B34" s="2">
         <v>174</v>
       </c>
-      <c r="C34" s="12">
+      <c r="C34" s="11">
         <v>56.26</v>
       </c>
       <c r="D34" t="s">
         <v>28</v>
       </c>
-      <c r="E34" s="9">
+      <c r="E34" s="8">
         <v>3147.3040000000001</v>
       </c>
-      <c r="F34" s="6">
+      <c r="F34" s="5">
         <f t="shared" si="0"/>
         <v>5268024</v>
       </c>
-      <c r="G34" s="5">
+      <c r="G34" s="4">
         <f t="shared" si="1"/>
         <v>0.59743539513107757</v>
       </c>
@@ -1855,20 +1861,20 @@
       <c r="B35" s="2">
         <v>199</v>
       </c>
-      <c r="C35" s="12">
+      <c r="C35" s="11">
         <v>53.54</v>
       </c>
       <c r="D35" t="s">
         <v>29</v>
       </c>
-      <c r="E35" s="9">
+      <c r="E35" s="8">
         <v>4727.4229999999998</v>
       </c>
-      <c r="F35" s="6">
+      <c r="F35" s="5">
         <f t="shared" si="0"/>
         <v>7880599</v>
       </c>
-      <c r="G35" s="5">
+      <c r="G35" s="4">
         <f t="shared" si="1"/>
         <v>0.59988117654508244</v>
       </c>
@@ -1880,20 +1886,20 @@
       <c r="B36" s="2">
         <v>224</v>
       </c>
-      <c r="C36" s="12">
+      <c r="C36" s="11">
         <v>54.93</v>
       </c>
       <c r="D36" t="s">
         <v>28</v>
       </c>
-      <c r="E36" s="9">
+      <c r="E36" s="8">
         <v>6846.9669999999996</v>
       </c>
-      <c r="F36" s="6">
+      <c r="F36" s="5">
         <f t="shared" si="0"/>
         <v>11239424</v>
       </c>
-      <c r="G36" s="5">
+      <c r="G36" s="4">
         <f t="shared" si="1"/>
         <v>0.6091919835037809</v>
       </c>
@@ -1905,20 +1911,20 @@
       <c r="B37" s="2">
         <v>249</v>
       </c>
-      <c r="C37" s="12">
+      <c r="C37" s="11">
         <v>53.89</v>
       </c>
       <c r="D37" t="s">
         <v>29</v>
       </c>
-      <c r="E37" s="9">
+      <c r="E37" s="8">
         <v>9444.9380000000001</v>
       </c>
-      <c r="F37" s="6">
+      <c r="F37" s="5">
         <f t="shared" si="0"/>
         <v>15438249</v>
       </c>
-      <c r="G37" s="5">
+      <c r="G37" s="4">
         <f t="shared" si="1"/>
         <v>0.61178816328198882</v>
       </c>
@@ -1930,20 +1936,20 @@
       <c r="B38" s="2">
         <v>274</v>
       </c>
-      <c r="C38" s="12">
+      <c r="C38" s="11">
         <v>53.84</v>
       </c>
       <c r="D38" t="s">
         <v>29</v>
       </c>
-      <c r="E38" s="9">
+      <c r="E38" s="8">
         <v>12392.65</v>
       </c>
-      <c r="F38" s="6">
+      <c r="F38" s="5">
         <f t="shared" si="0"/>
         <v>20570824</v>
       </c>
-      <c r="G38" s="5">
+      <c r="G38" s="4">
         <f t="shared" si="1"/>
         <v>0.60243819110017183</v>
       </c>
@@ -1955,20 +1961,20 @@
       <c r="B39" s="2">
         <v>299</v>
       </c>
-      <c r="C39" s="12">
+      <c r="C39" s="11">
         <v>59.36</v>
       </c>
       <c r="D39" t="s">
         <v>30</v>
       </c>
-      <c r="E39" s="9">
+      <c r="E39" s="8">
         <v>16180.44</v>
       </c>
-      <c r="F39" s="6">
+      <c r="F39" s="5">
         <f t="shared" si="0"/>
         <v>26730899</v>
       </c>
-      <c r="G39" s="5">
+      <c r="G39" s="4">
         <f t="shared" si="1"/>
         <v>0.60530848588369579</v>
       </c>
@@ -1980,20 +1986,20 @@
       <c r="B40" s="2">
         <v>324</v>
       </c>
-      <c r="C40" s="12">
+      <c r="C40" s="11">
         <v>62.17</v>
       </c>
       <c r="D40" t="s">
         <v>27</v>
       </c>
-      <c r="E40" s="9">
+      <c r="E40" s="8">
         <v>21234.156999999999</v>
       </c>
-      <c r="F40" s="6">
+      <c r="F40" s="5">
         <f t="shared" si="0"/>
         <v>34012224</v>
       </c>
-      <c r="G40" s="5">
+      <c r="G40" s="4">
         <f t="shared" si="1"/>
         <v>0.62430957175867119</v>
       </c>
@@ -2005,20 +2011,20 @@
       <c r="B41" s="2">
         <v>349</v>
       </c>
-      <c r="C41" s="12">
+      <c r="C41" s="11">
         <v>65.38</v>
       </c>
       <c r="D41" t="s">
         <v>31</v>
       </c>
-      <c r="E41" s="9">
+      <c r="E41" s="8">
         <v>26382.848999999998</v>
       </c>
-      <c r="F41" s="6">
+      <c r="F41" s="5">
         <f t="shared" si="0"/>
         <v>42508549</v>
       </c>
-      <c r="G41" s="5">
+      <c r="G41" s="4">
         <f t="shared" si="1"/>
         <v>0.62064807246184761</v>
       </c>
@@ -2030,20 +2036,20 @@
       <c r="B42" s="2">
         <v>374</v>
       </c>
-      <c r="C42" s="12">
+      <c r="C42" s="11">
         <v>48.82</v>
       </c>
       <c r="D42" t="s">
         <v>20</v>
       </c>
-      <c r="E42" s="9">
+      <c r="E42" s="8">
         <v>32421.217000000001</v>
       </c>
-      <c r="F42" s="6">
+      <c r="F42" s="5">
         <f t="shared" si="0"/>
         <v>52313624</v>
       </c>
-      <c r="G42" s="5">
+      <c r="G42" s="4">
         <f t="shared" si="1"/>
         <v>0.61974710450187886</v>
       </c>
@@ -2055,20 +2061,20 @@
       <c r="B43" s="2">
         <v>399</v>
       </c>
-      <c r="C43" s="12">
+      <c r="C43" s="11">
         <v>57.95</v>
       </c>
       <c r="D43" t="s">
         <v>26</v>
       </c>
-      <c r="E43" s="9">
+      <c r="E43" s="8">
         <v>39479.546000000002</v>
       </c>
-      <c r="F43" s="6">
+      <c r="F43" s="5">
         <f t="shared" si="0"/>
         <v>63521199</v>
       </c>
-      <c r="G43" s="5">
+      <c r="G43" s="4">
         <f t="shared" si="1"/>
         <v>0.62151764484168504</v>
       </c>
@@ -2080,20 +2086,20 @@
       <c r="B44" s="2">
         <v>424</v>
       </c>
-      <c r="C44" s="12">
+      <c r="C44" s="11">
         <v>63.7</v>
       </c>
       <c r="D44" t="s">
         <v>27</v>
       </c>
-      <c r="E44" s="9">
+      <c r="E44" s="8">
         <v>47759.883999999998</v>
       </c>
-      <c r="F44" s="6">
+      <c r="F44" s="5">
         <f t="shared" si="0"/>
         <v>76225024</v>
       </c>
-      <c r="G44" s="5">
+      <c r="G44" s="4">
         <f t="shared" si="1"/>
         <v>0.62656436815290473</v>
       </c>
@@ -2105,20 +2111,20 @@
       <c r="B45" s="2">
         <v>449</v>
       </c>
-      <c r="C45" s="12">
+      <c r="C45" s="11">
         <v>50.26</v>
       </c>
       <c r="D45" t="s">
         <v>22</v>
       </c>
-      <c r="E45" s="9">
+      <c r="E45" s="8">
         <v>56453.353000000003</v>
       </c>
-      <c r="F45" s="6">
+      <c r="F45" s="5">
         <f t="shared" si="0"/>
         <v>90518849</v>
       </c>
-      <c r="G45" s="5">
+      <c r="G45" s="4">
         <f t="shared" si="1"/>
         <v>0.62366406139344521</v>
       </c>
@@ -2130,20 +2136,20 @@
       <c r="B46" s="2">
         <v>474</v>
       </c>
-      <c r="C46" s="12">
+      <c r="C46" s="11">
         <v>54.55</v>
       </c>
       <c r="D46" t="s">
         <v>29</v>
       </c>
-      <c r="E46" s="9">
+      <c r="E46" s="8">
         <v>66522.074999999997</v>
       </c>
-      <c r="F46" s="6">
+      <c r="F46" s="5">
         <f t="shared" si="0"/>
         <v>106496424</v>
       </c>
-      <c r="G46" s="5">
+      <c r="G46" s="4">
         <f t="shared" si="1"/>
         <v>0.62464139640970473</v>
       </c>
@@ -2155,20 +2161,20 @@
       <c r="B47" s="2">
         <v>499</v>
       </c>
-      <c r="C47" s="12">
+      <c r="C47" s="11">
         <v>49.16</v>
       </c>
       <c r="D47" t="s">
         <v>20</v>
       </c>
-      <c r="E47" s="9">
+      <c r="E47" s="8">
         <v>78458.733999999997</v>
       </c>
-      <c r="F47" s="6">
+      <c r="F47" s="5">
         <f t="shared" si="0"/>
         <v>124251499</v>
       </c>
-      <c r="G47" s="5">
+      <c r="G47" s="4">
         <f t="shared" si="1"/>
         <v>0.63145100567358137</v>
       </c>
@@ -2180,20 +2186,20 @@
       <c r="B48" s="2">
         <v>524</v>
       </c>
-      <c r="C48" s="12">
+      <c r="C48" s="11">
         <v>55.46</v>
       </c>
       <c r="D48" t="s">
         <v>28</v>
       </c>
-      <c r="E48" s="9">
+      <c r="E48" s="8">
         <v>90990.404999999999</v>
       </c>
-      <c r="F48" s="6">
+      <c r="F48" s="5">
         <f t="shared" si="0"/>
         <v>143877824</v>
       </c>
-      <c r="G48" s="5">
+      <c r="G48" s="4">
         <f t="shared" si="1"/>
         <v>0.63241438096811908</v>
       </c>
@@ -2208,7 +2214,7 @@
   <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J32" sqref="J32"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2217,25 +2223,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="F1" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="G1" s="12" t="s">
         <v>13</v>
       </c>
     </row>
@@ -2243,7 +2249,7 @@
       <c r="A2" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="8">
+      <c r="B2" s="7">
         <v>24</v>
       </c>
       <c r="C2">
@@ -2252,14 +2258,14 @@
       <c r="D2" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="9">
+      <c r="E2" s="8">
         <v>0.42399999999999999</v>
       </c>
-      <c r="F2" s="6">
+      <c r="F2" s="5">
         <f>B2^2</f>
         <v>576</v>
       </c>
-      <c r="G2" s="5">
+      <c r="G2" s="4">
         <f>E2/F2*1000</f>
         <v>0.73611111111111105</v>
       </c>
@@ -2268,7 +2274,7 @@
       <c r="A3" t="s">
         <v>34</v>
       </c>
-      <c r="B3" s="8">
+      <c r="B3" s="7">
         <v>49</v>
       </c>
       <c r="C3">
@@ -2277,14 +2283,14 @@
       <c r="D3" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="9">
+      <c r="E3" s="8">
         <v>1.6479999999999999</v>
       </c>
-      <c r="F3" s="6">
+      <c r="F3" s="5">
         <f>B3^2</f>
         <v>2401</v>
       </c>
-      <c r="G3" s="5">
+      <c r="G3" s="4">
         <f t="shared" ref="G3:G22" si="0">E3/F3*1000</f>
         <v>0.6863806747188671</v>
       </c>
@@ -2293,7 +2299,7 @@
       <c r="A4" t="s">
         <v>34</v>
       </c>
-      <c r="B4" s="8">
+      <c r="B4" s="7">
         <v>74</v>
       </c>
       <c r="C4">
@@ -2302,14 +2308,14 @@
       <c r="D4" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="9">
+      <c r="E4" s="8">
         <v>3.6859999999999999</v>
       </c>
-      <c r="F4" s="6">
+      <c r="F4" s="5">
         <f t="shared" ref="F4:F22" si="1">B4^2</f>
         <v>5476</v>
       </c>
-      <c r="G4" s="5">
+      <c r="G4" s="4">
         <f t="shared" si="0"/>
         <v>0.67311906501095697</v>
       </c>
@@ -2318,7 +2324,7 @@
       <c r="A5" t="s">
         <v>34</v>
       </c>
-      <c r="B5" s="8">
+      <c r="B5" s="7">
         <v>99</v>
       </c>
       <c r="C5">
@@ -2327,14 +2333,14 @@
       <c r="D5" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="9">
+      <c r="E5" s="8">
         <v>6.5709999999999997</v>
       </c>
-      <c r="F5" s="6">
+      <c r="F5" s="5">
         <f t="shared" si="1"/>
         <v>9801</v>
       </c>
-      <c r="G5" s="5">
+      <c r="G5" s="4">
         <f t="shared" si="0"/>
         <v>0.67044179165391282</v>
       </c>
@@ -2343,7 +2349,7 @@
       <c r="A6" t="s">
         <v>34</v>
       </c>
-      <c r="B6" s="8">
+      <c r="B6" s="7">
         <v>124</v>
       </c>
       <c r="C6">
@@ -2352,14 +2358,14 @@
       <c r="D6" t="s">
         <v>28</v>
       </c>
-      <c r="E6" s="9">
+      <c r="E6" s="8">
         <v>10.064</v>
       </c>
-      <c r="F6" s="6">
+      <c r="F6" s="5">
         <f t="shared" si="1"/>
         <v>15376</v>
       </c>
-      <c r="G6" s="5">
+      <c r="G6" s="4">
         <f t="shared" si="0"/>
         <v>0.65452653485952139</v>
       </c>
@@ -2368,7 +2374,7 @@
       <c r="A7" t="s">
         <v>34</v>
       </c>
-      <c r="B7" s="8">
+      <c r="B7" s="7">
         <v>149</v>
       </c>
       <c r="C7">
@@ -2377,14 +2383,14 @@
       <c r="D7" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="9">
+      <c r="E7" s="8">
         <v>14.486000000000001</v>
       </c>
-      <c r="F7" s="6">
+      <c r="F7" s="5">
         <f t="shared" si="1"/>
         <v>22201</v>
       </c>
-      <c r="G7" s="5">
+      <c r="G7" s="4">
         <f t="shared" si="0"/>
         <v>0.65249313094004768</v>
       </c>
@@ -2393,7 +2399,7 @@
       <c r="A8" t="s">
         <v>34</v>
       </c>
-      <c r="B8" s="8">
+      <c r="B8" s="7">
         <v>174</v>
       </c>
       <c r="C8">
@@ -2402,14 +2408,14 @@
       <c r="D8" t="s">
         <v>28</v>
       </c>
-      <c r="E8" s="9">
+      <c r="E8" s="8">
         <v>20.148</v>
       </c>
-      <c r="F8" s="6">
+      <c r="F8" s="5">
         <f t="shared" si="1"/>
         <v>30276</v>
       </c>
-      <c r="G8" s="5">
+      <c r="G8" s="4">
         <f t="shared" si="0"/>
         <v>0.66547760602457384</v>
       </c>
@@ -2418,7 +2424,7 @@
       <c r="A9" t="s">
         <v>34</v>
       </c>
-      <c r="B9" s="8">
+      <c r="B9" s="7">
         <v>199</v>
       </c>
       <c r="C9">
@@ -2427,14 +2433,14 @@
       <c r="D9" t="s">
         <v>27</v>
       </c>
-      <c r="E9" s="9">
+      <c r="E9" s="8">
         <v>25.393999999999998</v>
       </c>
-      <c r="F9" s="6">
+      <c r="F9" s="5">
         <f t="shared" si="1"/>
         <v>39601</v>
       </c>
-      <c r="G9" s="5">
+      <c r="G9" s="4">
         <f t="shared" si="0"/>
         <v>0.64124643317087948</v>
       </c>
@@ -2443,7 +2449,7 @@
       <c r="A10" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="8">
+      <c r="B10" s="7">
         <v>224</v>
       </c>
       <c r="C10">
@@ -2452,14 +2458,14 @@
       <c r="D10" t="s">
         <v>28</v>
       </c>
-      <c r="E10" s="9">
+      <c r="E10" s="8">
         <v>32.317999999999998</v>
       </c>
-      <c r="F10" s="6">
+      <c r="F10" s="5">
         <f t="shared" si="1"/>
         <v>50176</v>
       </c>
-      <c r="G10" s="5">
+      <c r="G10" s="4">
         <f t="shared" si="0"/>
         <v>0.64409279336734693</v>
       </c>
@@ -2468,7 +2474,7 @@
       <c r="A11" t="s">
         <v>34</v>
       </c>
-      <c r="B11" s="8">
+      <c r="B11" s="7">
         <v>249</v>
       </c>
       <c r="C11">
@@ -2477,14 +2483,14 @@
       <c r="D11" t="s">
         <v>28</v>
       </c>
-      <c r="E11" s="9">
+      <c r="E11" s="8">
         <v>40.182000000000002</v>
       </c>
-      <c r="F11" s="6">
+      <c r="F11" s="5">
         <f t="shared" si="1"/>
         <v>62001</v>
       </c>
-      <c r="G11" s="5">
+      <c r="G11" s="4">
         <f t="shared" si="0"/>
         <v>0.64808632118836795</v>
       </c>
@@ -2493,7 +2499,7 @@
       <c r="A12" t="s">
         <v>34</v>
       </c>
-      <c r="B12" s="8">
+      <c r="B12" s="7">
         <v>274</v>
       </c>
       <c r="C12">
@@ -2502,14 +2508,14 @@
       <c r="D12" t="s">
         <v>25</v>
       </c>
-      <c r="E12" s="9">
+      <c r="E12" s="8">
         <v>47.276000000000003</v>
       </c>
-      <c r="F12" s="6">
+      <c r="F12" s="5">
         <f t="shared" si="1"/>
         <v>75076</v>
       </c>
-      <c r="G12" s="5">
+      <c r="G12" s="4">
         <f t="shared" si="0"/>
         <v>0.62970856199051628</v>
       </c>
@@ -2518,7 +2524,7 @@
       <c r="A13" t="s">
         <v>34</v>
       </c>
-      <c r="B13" s="8">
+      <c r="B13" s="7">
         <v>299</v>
       </c>
       <c r="C13">
@@ -2527,14 +2533,14 @@
       <c r="D13" t="s">
         <v>30</v>
       </c>
-      <c r="E13" s="9">
+      <c r="E13" s="8">
         <v>56.856000000000002</v>
       </c>
-      <c r="F13" s="6">
+      <c r="F13" s="5">
         <f t="shared" si="1"/>
         <v>89401</v>
       </c>
-      <c r="G13" s="5">
+      <c r="G13" s="4">
         <f t="shared" si="0"/>
         <v>0.63596604064831486</v>
       </c>
@@ -2543,7 +2549,7 @@
       <c r="A14" t="s">
         <v>34</v>
       </c>
-      <c r="B14" s="8">
+      <c r="B14" s="7">
         <v>324</v>
       </c>
       <c r="C14">
@@ -2552,14 +2558,14 @@
       <c r="D14" t="s">
         <v>30</v>
       </c>
-      <c r="E14" s="9">
+      <c r="E14" s="8">
         <v>65.701999999999998</v>
       </c>
-      <c r="F14" s="6">
+      <c r="F14" s="5">
         <f t="shared" si="1"/>
         <v>104976</v>
       </c>
-      <c r="G14" s="5">
+      <c r="G14" s="4">
         <f t="shared" si="0"/>
         <v>0.6258763907940863</v>
       </c>
@@ -2568,7 +2574,7 @@
       <c r="A15" t="s">
         <v>34</v>
       </c>
-      <c r="B15" s="8">
+      <c r="B15" s="7">
         <v>349</v>
       </c>
       <c r="C15">
@@ -2577,14 +2583,14 @@
       <c r="D15" t="s">
         <v>20</v>
       </c>
-      <c r="E15" s="9">
+      <c r="E15" s="8">
         <v>78.305999999999997</v>
       </c>
-      <c r="F15" s="6">
+      <c r="F15" s="5">
         <f t="shared" si="1"/>
         <v>121801</v>
       </c>
-      <c r="G15" s="5">
+      <c r="G15" s="4">
         <f t="shared" si="0"/>
         <v>0.64290112560652213</v>
       </c>
@@ -2593,7 +2599,7 @@
       <c r="A16" t="s">
         <v>34</v>
       </c>
-      <c r="B16" s="8">
+      <c r="B16" s="7">
         <v>374</v>
       </c>
       <c r="C16">
@@ -2602,14 +2608,14 @@
       <c r="D16" t="s">
         <v>32</v>
       </c>
-      <c r="E16" s="9">
+      <c r="E16" s="8">
         <v>93.004000000000005</v>
       </c>
-      <c r="F16" s="6">
+      <c r="F16" s="5">
         <f t="shared" si="1"/>
         <v>139876</v>
       </c>
-      <c r="G16" s="5">
+      <c r="G16" s="4">
         <f t="shared" si="0"/>
         <v>0.66490319997712266</v>
       </c>
@@ -2618,7 +2624,7 @@
       <c r="A17" t="s">
         <v>34</v>
       </c>
-      <c r="B17" s="8">
+      <c r="B17" s="7">
         <v>399</v>
       </c>
       <c r="C17">
@@ -2627,14 +2633,14 @@
       <c r="D17" t="s">
         <v>30</v>
       </c>
-      <c r="E17" s="9">
+      <c r="E17" s="8">
         <v>104.417</v>
       </c>
-      <c r="F17" s="6">
+      <c r="F17" s="5">
         <f t="shared" si="1"/>
         <v>159201</v>
       </c>
-      <c r="G17" s="5">
+      <c r="G17" s="4">
         <f t="shared" si="0"/>
         <v>0.65588155853292374</v>
       </c>
@@ -2643,7 +2649,7 @@
       <c r="A18" t="s">
         <v>34</v>
       </c>
-      <c r="B18" s="8">
+      <c r="B18" s="7">
         <v>424</v>
       </c>
       <c r="C18">
@@ -2652,14 +2658,14 @@
       <c r="D18" t="s">
         <v>27</v>
       </c>
-      <c r="E18" s="9">
+      <c r="E18" s="8">
         <v>119.071</v>
       </c>
-      <c r="F18" s="6">
+      <c r="F18" s="5">
         <f t="shared" si="1"/>
         <v>179776</v>
       </c>
-      <c r="G18" s="5">
+      <c r="G18" s="4">
         <f t="shared" si="0"/>
         <v>0.6623297881808472</v>
       </c>
@@ -2668,7 +2674,7 @@
       <c r="A19" t="s">
         <v>34</v>
       </c>
-      <c r="B19" s="8">
+      <c r="B19" s="7">
         <v>449</v>
       </c>
       <c r="C19">
@@ -2677,14 +2683,14 @@
       <c r="D19" t="s">
         <v>31</v>
       </c>
-      <c r="E19" s="9">
+      <c r="E19" s="8">
         <v>141.10900000000001</v>
       </c>
-      <c r="F19" s="6">
+      <c r="F19" s="5">
         <f t="shared" si="1"/>
         <v>201601</v>
       </c>
-      <c r="G19" s="5">
+      <c r="G19" s="4">
         <f t="shared" si="0"/>
         <v>0.69994196457358848</v>
       </c>
@@ -2693,7 +2699,7 @@
       <c r="A20" t="s">
         <v>34</v>
       </c>
-      <c r="B20" s="8">
+      <c r="B20" s="7">
         <v>474</v>
       </c>
       <c r="C20">
@@ -2702,14 +2708,14 @@
       <c r="D20" t="s">
         <v>32</v>
       </c>
-      <c r="E20" s="9">
+      <c r="E20" s="8">
         <v>145.678</v>
       </c>
-      <c r="F20" s="6">
+      <c r="F20" s="5">
         <f t="shared" si="1"/>
         <v>224676</v>
       </c>
-      <c r="G20" s="5">
+      <c r="G20" s="4">
         <f t="shared" si="0"/>
         <v>0.6483914614823123</v>
       </c>
@@ -2718,7 +2724,7 @@
       <c r="A21" t="s">
         <v>34</v>
       </c>
-      <c r="B21" s="8">
+      <c r="B21" s="7">
         <v>499</v>
       </c>
       <c r="C21">
@@ -2727,14 +2733,14 @@
       <c r="D21" t="s">
         <v>31</v>
       </c>
-      <c r="E21" s="9">
+      <c r="E21" s="8">
         <v>167.845</v>
       </c>
-      <c r="F21" s="6">
+      <c r="F21" s="5">
         <f t="shared" si="1"/>
         <v>249001</v>
       </c>
-      <c r="G21" s="5">
+      <c r="G21" s="4">
         <f t="shared" si="0"/>
         <v>0.6740735980979996</v>
       </c>
@@ -2743,7 +2749,7 @@
       <c r="A22" t="s">
         <v>34</v>
       </c>
-      <c r="B22" s="8">
+      <c r="B22" s="7">
         <v>524</v>
       </c>
       <c r="C22">
@@ -2752,14 +2758,14 @@
       <c r="D22" t="s">
         <v>33</v>
       </c>
-      <c r="E22" s="9">
+      <c r="E22" s="8">
         <v>185.93100000000001</v>
       </c>
-      <c r="F22" s="6">
+      <c r="F22" s="5">
         <f t="shared" si="1"/>
         <v>274576</v>
       </c>
-      <c r="G22" s="5">
+      <c r="G22" s="4">
         <f t="shared" si="0"/>
         <v>0.67715677990793077</v>
       </c>
@@ -2774,7 +2780,7 @@
   <dimension ref="A1:V43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K25" sqref="K25"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2782,75 +2788,76 @@
     <col min="1" max="1" width="7.28515625" customWidth="1"/>
     <col min="3" max="3" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" style="8" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="9.28515625" customWidth="1"/>
+    <col min="22" max="22" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:22" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="H1" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="J1" s="10" t="s">
+      <c r="J1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="K1" s="10" t="s">
+      <c r="K1" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="L1" s="10" t="s">
+      <c r="L1" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="M1" s="10" t="s">
+      <c r="M1" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="N1" s="10" t="s">
+      <c r="N1" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="O1" s="10" t="s">
+      <c r="O1" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="P1" s="10" t="s">
+      <c r="P1" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="Q1" s="10" t="s">
+      <c r="Q1" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="S1" s="10" t="s">
+      <c r="S1" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="T1" s="10" t="s">
+      <c r="T1" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="U1" s="10" t="s">
+      <c r="U1" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="V1" s="10" t="s">
+      <c r="V1" s="9" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A2" s="8">
+      <c r="A2" s="7">
         <v>24</v>
       </c>
       <c r="B2">
@@ -2862,7 +2869,7 @@
       <c r="D2" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="9">
+      <c r="E2" s="8">
         <v>0.42399999999999999</v>
       </c>
       <c r="F2">
@@ -2877,7 +2884,7 @@
         <f>B2-B3</f>
         <v>0</v>
       </c>
-      <c r="J2" s="8">
+      <c r="J2" s="7">
         <v>24</v>
       </c>
       <c r="K2">
@@ -2904,7 +2911,7 @@
         <f>O2-N2</f>
         <v>0</v>
       </c>
-      <c r="Q2" s="16">
+      <c r="Q2" s="15">
         <f>P2/O2</f>
         <v>0</v>
       </c>
@@ -2915,17 +2922,17 @@
         <f>COUNTIF($M$2:$M$22,S2)</f>
         <v>13</v>
       </c>
-      <c r="U2" s="12">
+      <c r="U2" s="11">
         <f>AVERAGEIF($M$2:$M$22,$S2,P2:P22)</f>
         <v>8.6461538461538474</v>
       </c>
-      <c r="V2" s="16">
+      <c r="V2" s="15">
         <f>AVERAGEIF($M$2:$M$22,$S2,Q2:Q22)</f>
         <v>0.13281277531046884</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A3" s="8">
+      <c r="A3" s="7">
         <v>24</v>
       </c>
       <c r="B3">
@@ -2937,14 +2944,14 @@
       <c r="D3" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="9">
+      <c r="E3" s="8">
         <v>7.9969999999999999</v>
       </c>
-      <c r="H3" s="16">
+      <c r="H3" s="15">
         <f>B2/B3</f>
         <v>1</v>
       </c>
-      <c r="J3" s="8">
+      <c r="J3" s="7">
         <v>49</v>
       </c>
       <c r="K3">
@@ -2971,7 +2978,7 @@
         <f t="shared" ref="P3:P22" si="3">O3-N3</f>
         <v>3.6299999999999955</v>
       </c>
-      <c r="Q3" s="16">
+      <c r="Q3" s="15">
         <f t="shared" ref="Q3:Q22" si="4">P3/O3</f>
         <v>6.0019841269841195E-2</v>
       </c>
@@ -2982,17 +2989,17 @@
         <f>COUNTIF($M$2:$M$22,S3)</f>
         <v>7</v>
       </c>
-      <c r="U3" s="12">
+      <c r="U3" s="11">
         <f>AVERAGEIF($M$2:$M$22,$S3,P2:P22)</f>
         <v>5.5114285714285716</v>
       </c>
-      <c r="V3" s="16">
+      <c r="V3" s="15">
         <f>AVERAGEIF($M$2:$M$22,$S3,Q3:Q23)</f>
         <v>0.16894501631810033</v>
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A4" s="8">
+      <c r="A4" s="7">
         <v>49</v>
       </c>
       <c r="B4">
@@ -3004,7 +3011,7 @@
       <c r="D4" t="s">
         <v>25</v>
       </c>
-      <c r="E4" s="9">
+      <c r="E4" s="8">
         <v>1.6479999999999999</v>
       </c>
       <c r="F4">
@@ -3019,7 +3026,7 @@
         <f t="shared" ref="H4" si="5">B4-B5</f>
         <v>3.6299999999999955</v>
       </c>
-      <c r="J4" s="8">
+      <c r="J4" s="7">
         <v>74</v>
       </c>
       <c r="K4">
@@ -3046,7 +3053,7 @@
         <f t="shared" si="3"/>
         <v>11.04</v>
       </c>
-      <c r="Q4" s="16">
+      <c r="Q4" s="15">
         <f t="shared" si="4"/>
         <v>0.17916260954235638</v>
       </c>
@@ -3063,7 +3070,7 @@
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A5" s="8">
+      <c r="A5" s="7">
         <v>49</v>
       </c>
       <c r="B5">
@@ -3075,14 +3082,14 @@
       <c r="D5" t="s">
         <v>26</v>
       </c>
-      <c r="E5" s="9">
+      <c r="E5" s="8">
         <v>69.635000000000005</v>
       </c>
-      <c r="H5" s="16">
+      <c r="H5" s="15">
         <f t="shared" ref="H5" si="8">B4/B5</f>
         <v>1.0638522427440633</v>
       </c>
-      <c r="J5" s="8">
+      <c r="J5" s="7">
         <v>99</v>
       </c>
       <c r="K5">
@@ -3109,13 +3116,13 @@
         <f t="shared" si="3"/>
         <v>11.900000000000006</v>
       </c>
-      <c r="Q5" s="16">
+      <c r="Q5" s="15">
         <f t="shared" si="4"/>
         <v>0.18713634219216865</v>
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A6" s="8">
+      <c r="A6" s="7">
         <v>74</v>
       </c>
       <c r="B6">
@@ -3127,7 +3134,7 @@
       <c r="D6" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="9">
+      <c r="E6" s="8">
         <v>3.6859999999999999</v>
       </c>
       <c r="F6">
@@ -3142,7 +3149,7 @@
         <f t="shared" ref="H6" si="9">B6-B7</f>
         <v>-11.04</v>
       </c>
-      <c r="J6" s="8">
+      <c r="J6" s="7">
         <v>124</v>
       </c>
       <c r="K6">
@@ -3169,13 +3176,13 @@
         <f t="shared" si="3"/>
         <v>2.2100000000000009</v>
       </c>
-      <c r="Q6" s="16">
+      <c r="Q6" s="15">
         <f t="shared" si="4"/>
         <v>3.8481629810203741E-2</v>
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A7" s="8">
+      <c r="A7" s="7">
         <v>74</v>
       </c>
       <c r="B7">
@@ -3187,14 +3194,14 @@
       <c r="D7" t="s">
         <v>25</v>
       </c>
-      <c r="E7" s="9">
+      <c r="E7" s="8">
         <v>242.64599999999999</v>
       </c>
-      <c r="H7" s="16">
+      <c r="H7" s="15">
         <f t="shared" ref="H7" si="10">B6/B7</f>
         <v>0.82083739045764359</v>
       </c>
-      <c r="J7" s="8">
+      <c r="J7" s="7">
         <v>149</v>
       </c>
       <c r="K7">
@@ -3221,13 +3228,13 @@
         <f t="shared" si="3"/>
         <v>3.9500000000000028</v>
       </c>
-      <c r="Q7" s="16">
+      <c r="Q7" s="15">
         <f t="shared" si="4"/>
         <v>7.0864729099390067E-2</v>
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A8" s="8">
+      <c r="A8" s="7">
         <v>99</v>
       </c>
       <c r="B8">
@@ -3239,7 +3246,7 @@
       <c r="D8" t="s">
         <v>27</v>
       </c>
-      <c r="E8" s="9">
+      <c r="E8" s="8">
         <v>6.5709999999999997</v>
       </c>
       <c r="F8">
@@ -3254,7 +3261,7 @@
         <f t="shared" ref="H8" si="11">B8-B9</f>
         <v>11.900000000000006</v>
       </c>
-      <c r="J8" s="8">
+      <c r="J8" s="7">
         <v>174</v>
       </c>
       <c r="K8">
@@ -3281,13 +3288,13 @@
         <f t="shared" si="3"/>
         <v>0.47999999999999687</v>
       </c>
-      <c r="Q8" s="16">
+      <c r="Q8" s="15">
         <f t="shared" si="4"/>
         <v>8.5318165659437773E-3</v>
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A9" s="8">
+      <c r="A9" s="7">
         <v>99</v>
       </c>
       <c r="B9">
@@ -3299,14 +3306,14 @@
       <c r="D9" t="s">
         <v>21</v>
       </c>
-      <c r="E9" s="9">
+      <c r="E9" s="8">
         <v>580.61199999999997</v>
       </c>
-      <c r="H9" s="16">
+      <c r="H9" s="15">
         <f t="shared" ref="H9" si="12">B8/B9</f>
         <v>1.2302186109498938</v>
       </c>
-      <c r="J9" s="8">
+      <c r="J9" s="7">
         <v>199</v>
       </c>
       <c r="K9">
@@ -3333,13 +3340,13 @@
         <f t="shared" si="3"/>
         <v>9.9100000000000037</v>
       </c>
-      <c r="Q9" s="16">
+      <c r="Q9" s="15">
         <f t="shared" si="4"/>
         <v>0.15618597320724986</v>
       </c>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A10" s="8">
+      <c r="A10" s="7">
         <v>124</v>
       </c>
       <c r="B10">
@@ -3351,7 +3358,7 @@
       <c r="D10" t="s">
         <v>28</v>
       </c>
-      <c r="E10" s="9">
+      <c r="E10" s="8">
         <v>10.064</v>
       </c>
       <c r="F10">
@@ -3366,7 +3373,7 @@
         <f t="shared" ref="H10" si="13">B10-B11</f>
         <v>-2.2100000000000009</v>
       </c>
-      <c r="J10" s="8">
+      <c r="J10" s="7">
         <v>224</v>
       </c>
       <c r="K10">
@@ -3393,13 +3400,13 @@
         <f t="shared" si="3"/>
         <v>0.46999999999999886</v>
       </c>
-      <c r="Q10" s="16">
+      <c r="Q10" s="15">
         <f t="shared" si="4"/>
         <v>8.4837545126353591E-3</v>
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A11" s="8">
+      <c r="A11" s="7">
         <v>124</v>
       </c>
       <c r="B11">
@@ -3411,14 +3418,14 @@
       <c r="D11" t="s">
         <v>26</v>
       </c>
-      <c r="E11" s="9">
+      <c r="E11" s="8">
         <v>1083.5719999999999</v>
       </c>
-      <c r="H11" s="16">
+      <c r="H11" s="15">
         <f t="shared" ref="H11" si="14">B10/B11</f>
         <v>0.96151837018979625</v>
       </c>
-      <c r="J11" s="8">
+      <c r="J11" s="7">
         <v>249</v>
       </c>
       <c r="K11">
@@ -3445,13 +3452,13 @@
         <f t="shared" si="3"/>
         <v>2.269999999999996</v>
       </c>
-      <c r="Q11" s="16">
+      <c r="Q11" s="15">
         <f t="shared" si="4"/>
         <v>4.0420227920227855E-2</v>
       </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A12" s="8">
+      <c r="A12" s="7">
         <v>149</v>
       </c>
       <c r="B12">
@@ -3463,7 +3470,7 @@
       <c r="D12" t="s">
         <v>21</v>
       </c>
-      <c r="E12" s="9">
+      <c r="E12" s="8">
         <v>14.486000000000001</v>
       </c>
       <c r="F12">
@@ -3478,7 +3485,7 @@
         <f t="shared" ref="H12" si="15">B12-B13</f>
         <v>-3.9500000000000028</v>
       </c>
-      <c r="J12" s="8">
+      <c r="J12" s="7">
         <v>274</v>
       </c>
       <c r="K12">
@@ -3505,13 +3512,13 @@
         <f t="shared" si="3"/>
         <v>7.8599999999999994</v>
       </c>
-      <c r="Q12" s="16">
+      <c r="Q12" s="15">
         <f t="shared" si="4"/>
         <v>0.12739059967585087</v>
       </c>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A13" s="8">
+      <c r="A13" s="7">
         <v>149</v>
       </c>
       <c r="B13">
@@ -3523,14 +3530,14 @@
       <c r="D13" t="s">
         <v>28</v>
       </c>
-      <c r="E13" s="9">
+      <c r="E13" s="8">
         <v>1952.914</v>
       </c>
-      <c r="H13" s="16">
+      <c r="H13" s="15">
         <f t="shared" ref="H13" si="16">B12/B13</f>
         <v>0.92913527090060988</v>
       </c>
-      <c r="J13" s="8">
+      <c r="J13" s="7">
         <v>299</v>
       </c>
       <c r="K13">
@@ -3557,13 +3564,13 @@
         <f t="shared" si="3"/>
         <v>0.31000000000000227</v>
       </c>
-      <c r="Q13" s="16">
+      <c r="Q13" s="15">
         <f t="shared" si="4"/>
         <v>5.195240489358174E-3</v>
       </c>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A14" s="8">
+      <c r="A14" s="7">
         <v>174</v>
       </c>
       <c r="B14">
@@ -3575,7 +3582,7 @@
       <c r="D14" t="s">
         <v>28</v>
       </c>
-      <c r="E14" s="9">
+      <c r="E14" s="8">
         <v>20.148</v>
       </c>
       <c r="F14">
@@ -3590,7 +3597,7 @@
         <f t="shared" ref="H14" si="17">B14-B15</f>
         <v>-0.47999999999999687</v>
       </c>
-      <c r="J14" s="8">
+      <c r="J14" s="7">
         <v>324</v>
       </c>
       <c r="K14">
@@ -3617,13 +3624,13 @@
         <f t="shared" si="3"/>
         <v>3</v>
       </c>
-      <c r="Q14" s="16">
+      <c r="Q14" s="15">
         <f t="shared" si="4"/>
         <v>4.8254785266205566E-2</v>
       </c>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A15" s="8">
+      <c r="A15" s="7">
         <v>174</v>
       </c>
       <c r="B15">
@@ -3635,14 +3642,14 @@
       <c r="D15" t="s">
         <v>28</v>
       </c>
-      <c r="E15" s="9">
+      <c r="E15" s="8">
         <v>3147.3040000000001</v>
       </c>
-      <c r="H15" s="16">
+      <c r="H15" s="15">
         <f t="shared" ref="H15" si="18">B14/B15</f>
         <v>0.99146818343405618</v>
       </c>
-      <c r="J15" s="8">
+      <c r="J15" s="7">
         <v>349</v>
       </c>
       <c r="K15">
@@ -3669,13 +3676,13 @@
         <f t="shared" si="3"/>
         <v>16.489999999999995</v>
       </c>
-      <c r="Q15" s="16">
+      <c r="Q15" s="15">
         <f t="shared" si="4"/>
         <v>0.2522178036096665</v>
       </c>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A16" s="8">
+      <c r="A16" s="7">
         <v>199</v>
       </c>
       <c r="B16">
@@ -3687,7 +3694,7 @@
       <c r="D16" t="s">
         <v>27</v>
       </c>
-      <c r="E16" s="9">
+      <c r="E16" s="8">
         <v>25.393999999999998</v>
       </c>
       <c r="F16">
@@ -3702,7 +3709,7 @@
         <f t="shared" ref="H16" si="19">B16-B17</f>
         <v>9.9100000000000037</v>
       </c>
-      <c r="J16" s="8">
+      <c r="J16" s="7">
         <v>374</v>
       </c>
       <c r="K16">
@@ -3729,13 +3736,13 @@
         <f t="shared" si="3"/>
         <v>19.770000000000003</v>
       </c>
-      <c r="Q16" s="16">
+      <c r="Q16" s="15">
         <f t="shared" si="4"/>
         <v>0.28823443650677943</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A17" s="8">
+      <c r="A17" s="7">
         <v>199</v>
       </c>
       <c r="B17">
@@ -3747,14 +3754,14 @@
       <c r="D17" t="s">
         <v>29</v>
       </c>
-      <c r="E17" s="9">
+      <c r="E17" s="8">
         <v>4727.4229999999998</v>
       </c>
-      <c r="H17" s="16">
+      <c r="H17" s="15">
         <f t="shared" ref="H17" si="20">B16/B17</f>
         <v>1.1850952558834518</v>
       </c>
-      <c r="J17" s="8">
+      <c r="J17" s="7">
         <v>399</v>
       </c>
       <c r="K17">
@@ -3781,13 +3788,13 @@
         <f t="shared" si="3"/>
         <v>1.009999999999998</v>
       </c>
-      <c r="Q17" s="16">
+      <c r="Q17" s="15">
         <f t="shared" si="4"/>
         <v>1.713025780189956E-2</v>
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A18" s="8">
+      <c r="A18" s="7">
         <v>224</v>
       </c>
       <c r="B18">
@@ -3799,7 +3806,7 @@
       <c r="D18" t="s">
         <v>28</v>
       </c>
-      <c r="E18" s="9">
+      <c r="E18" s="8">
         <v>32.317999999999998</v>
       </c>
       <c r="F18">
@@ -3814,7 +3821,7 @@
         <f t="shared" ref="H18" si="21">B18-B19</f>
         <v>0.46999999999999886</v>
       </c>
-      <c r="J18" s="8">
+      <c r="J18" s="7">
         <v>424</v>
       </c>
       <c r="K18">
@@ -3841,13 +3848,13 @@
         <f t="shared" si="3"/>
         <v>1.4100000000000037</v>
       </c>
-      <c r="Q18" s="16">
+      <c r="Q18" s="15">
         <f t="shared" si="4"/>
         <v>2.213500784929362E-2</v>
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A19" s="8">
+      <c r="A19" s="7">
         <v>224</v>
       </c>
       <c r="B19">
@@ -3859,14 +3866,14 @@
       <c r="D19" t="s">
         <v>28</v>
       </c>
-      <c r="E19" s="9">
+      <c r="E19" s="8">
         <v>6846.9669999999996</v>
       </c>
-      <c r="H19" s="16">
+      <c r="H19" s="15">
         <f t="shared" ref="H19" si="22">B18/B19</f>
         <v>1.0085563444383761</v>
       </c>
-      <c r="J19" s="8">
+      <c r="J19" s="7">
         <v>449</v>
       </c>
       <c r="K19">
@@ -3893,13 +3900,13 @@
         <f t="shared" si="3"/>
         <v>14.130000000000003</v>
       </c>
-      <c r="Q19" s="16">
+      <c r="Q19" s="15">
         <f t="shared" si="4"/>
         <v>0.21944401304550401</v>
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A20" s="8">
+      <c r="A20" s="7">
         <v>249</v>
       </c>
       <c r="B20">
@@ -3911,7 +3918,7 @@
       <c r="D20" t="s">
         <v>28</v>
       </c>
-      <c r="E20" s="9">
+      <c r="E20" s="8">
         <v>40.182000000000002</v>
       </c>
       <c r="F20">
@@ -3926,7 +3933,7 @@
         <f t="shared" ref="H20" si="23">B20-B21</f>
         <v>2.269999999999996</v>
       </c>
-      <c r="J20" s="8">
+      <c r="J20" s="7">
         <v>474</v>
       </c>
       <c r="K20">
@@ -3953,13 +3960,13 @@
         <f t="shared" si="3"/>
         <v>13.600000000000009</v>
       </c>
-      <c r="Q20" s="16">
+      <c r="Q20" s="15">
         <f t="shared" si="4"/>
         <v>0.19955979457079981</v>
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A21" s="8">
+      <c r="A21" s="7">
         <v>249</v>
       </c>
       <c r="B21">
@@ -3971,14 +3978,14 @@
       <c r="D21" t="s">
         <v>29</v>
       </c>
-      <c r="E21" s="9">
+      <c r="E21" s="8">
         <v>9444.9380000000001</v>
       </c>
-      <c r="H21" s="16">
+      <c r="H21" s="15">
         <f t="shared" ref="H21" si="24">B20/B21</f>
         <v>1.042122842827983</v>
       </c>
-      <c r="J21" s="8">
+      <c r="J21" s="7">
         <v>499</v>
       </c>
       <c r="K21">
@@ -4005,13 +4012,13 @@
         <f t="shared" si="3"/>
         <v>16.450000000000003</v>
       </c>
-      <c r="Q21" s="16">
+      <c r="Q21" s="15">
         <f t="shared" si="4"/>
         <v>0.25072397500381044</v>
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A22" s="8">
+      <c r="A22" s="7">
         <v>274</v>
       </c>
       <c r="B22">
@@ -4023,7 +4030,7 @@
       <c r="D22" t="s">
         <v>25</v>
       </c>
-      <c r="E22" s="9">
+      <c r="E22" s="8">
         <v>47.276000000000003</v>
       </c>
       <c r="F22">
@@ -4038,7 +4045,7 @@
         <f t="shared" ref="H22" si="25">B22-B23</f>
         <v>7.8599999999999994</v>
       </c>
-      <c r="J22" s="8">
+      <c r="J22" s="7">
         <v>524</v>
       </c>
       <c r="K22">
@@ -4065,13 +4072,13 @@
         <f t="shared" si="3"/>
         <v>11.089999999999996</v>
       </c>
-      <c r="Q22" s="16">
+      <c r="Q22" s="15">
         <f t="shared" si="4"/>
         <v>0.16664162283996989</v>
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A23" s="8">
+      <c r="A23" s="7">
         <v>274</v>
       </c>
       <c r="B23">
@@ -4083,16 +4090,16 @@
       <c r="D23" t="s">
         <v>29</v>
       </c>
-      <c r="E23" s="9">
+      <c r="E23" s="8">
         <v>12392.65</v>
       </c>
-      <c r="H23" s="16">
+      <c r="H23" s="15">
         <f t="shared" ref="H23" si="26">B22/B23</f>
         <v>1.1459881129271916</v>
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A24" s="8">
+      <c r="A24" s="7">
         <v>299</v>
       </c>
       <c r="B24">
@@ -4104,7 +4111,7 @@
       <c r="D24" t="s">
         <v>30</v>
       </c>
-      <c r="E24" s="9">
+      <c r="E24" s="8">
         <v>56.856000000000002</v>
       </c>
       <c r="F24">
@@ -4121,7 +4128,7 @@
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A25" s="8">
+      <c r="A25" s="7">
         <v>299</v>
       </c>
       <c r="B25">
@@ -4133,16 +4140,16 @@
       <c r="D25" t="s">
         <v>30</v>
       </c>
-      <c r="E25" s="9">
+      <c r="E25" s="8">
         <v>16180.44</v>
       </c>
-      <c r="H25" s="16">
+      <c r="H25" s="15">
         <f t="shared" ref="H25" si="28">B24/B25</f>
         <v>1.005222371967655</v>
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A26" s="8">
+      <c r="A26" s="7">
         <v>324</v>
       </c>
       <c r="B26">
@@ -4154,7 +4161,7 @@
       <c r="D26" t="s">
         <v>30</v>
       </c>
-      <c r="E26" s="9">
+      <c r="E26" s="8">
         <v>65.701999999999998</v>
       </c>
       <c r="F26">
@@ -4171,7 +4178,7 @@
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A27" s="8">
+      <c r="A27" s="7">
         <v>324</v>
       </c>
       <c r="B27">
@@ -4183,16 +4190,16 @@
       <c r="D27" t="s">
         <v>27</v>
       </c>
-      <c r="E27" s="9">
+      <c r="E27" s="8">
         <v>21234.156999999999</v>
       </c>
-      <c r="H27" s="16">
+      <c r="H27" s="15">
         <f t="shared" ref="H27" si="30">B26/B27</f>
         <v>0.95174521473379448</v>
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A28" s="8">
+      <c r="A28" s="7">
         <v>349</v>
       </c>
       <c r="B28">
@@ -4204,7 +4211,7 @@
       <c r="D28" t="s">
         <v>20</v>
       </c>
-      <c r="E28" s="9">
+      <c r="E28" s="8">
         <v>78.305999999999997</v>
       </c>
       <c r="F28">
@@ -4221,7 +4228,7 @@
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A29" s="8">
+      <c r="A29" s="7">
         <v>349</v>
       </c>
       <c r="B29">
@@ -4233,16 +4240,16 @@
       <c r="D29" t="s">
         <v>31</v>
       </c>
-      <c r="E29" s="9">
+      <c r="E29" s="8">
         <v>26382.848999999998</v>
       </c>
-      <c r="H29" s="16">
+      <c r="H29" s="15">
         <f t="shared" ref="H29:H43" si="32">B28/B29</f>
         <v>0.7477821963903335</v>
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A30" s="8">
+      <c r="A30" s="7">
         <v>374</v>
       </c>
       <c r="B30">
@@ -4254,7 +4261,7 @@
       <c r="D30" t="s">
         <v>32</v>
       </c>
-      <c r="E30" s="9">
+      <c r="E30" s="8">
         <v>93.004000000000005</v>
       </c>
       <c r="F30">
@@ -4271,7 +4278,7 @@
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A31" s="8">
+      <c r="A31" s="7">
         <v>374</v>
       </c>
       <c r="B31">
@@ -4283,16 +4290,16 @@
       <c r="D31" t="s">
         <v>20</v>
       </c>
-      <c r="E31" s="9">
+      <c r="E31" s="8">
         <v>32421.217000000001</v>
       </c>
-      <c r="H31" s="16">
+      <c r="H31" s="15">
         <f t="shared" ref="H31:H43" si="34">B30/B31</f>
         <v>1.4049569848422778</v>
       </c>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A32" s="8">
+      <c r="A32" s="7">
         <v>399</v>
       </c>
       <c r="B32">
@@ -4304,7 +4311,7 @@
       <c r="D32" t="s">
         <v>30</v>
       </c>
-      <c r="E32" s="9">
+      <c r="E32" s="8">
         <v>104.417</v>
       </c>
       <c r="F32">
@@ -4321,7 +4328,7 @@
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="8">
+      <c r="A33" s="7">
         <v>399</v>
       </c>
       <c r="B33">
@@ -4333,16 +4340,16 @@
       <c r="D33" t="s">
         <v>26</v>
       </c>
-      <c r="E33" s="9">
+      <c r="E33" s="8">
         <v>39479.546000000002</v>
       </c>
-      <c r="H33" s="16">
+      <c r="H33" s="15">
         <f t="shared" ref="H33:H43" si="36">B32/B33</f>
         <v>1.0174288179465056</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="8">
+      <c r="A34" s="7">
         <v>424</v>
       </c>
       <c r="B34">
@@ -4354,7 +4361,7 @@
       <c r="D34" t="s">
         <v>27</v>
       </c>
-      <c r="E34" s="9">
+      <c r="E34" s="8">
         <v>119.071</v>
       </c>
       <c r="F34">
@@ -4371,7 +4378,7 @@
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="8">
+      <c r="A35" s="7">
         <v>424</v>
       </c>
       <c r="B35">
@@ -4383,16 +4390,16 @@
       <c r="D35" t="s">
         <v>27</v>
       </c>
-      <c r="E35" s="9">
+      <c r="E35" s="8">
         <v>47759.883999999998</v>
       </c>
-      <c r="H35" s="16">
+      <c r="H35" s="15">
         <f t="shared" ref="H35:H43" si="38">B34/B35</f>
         <v>0.97786499215070632</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="8">
+      <c r="A36" s="7">
         <v>449</v>
       </c>
       <c r="B36">
@@ -4404,7 +4411,7 @@
       <c r="D36" t="s">
         <v>31</v>
       </c>
-      <c r="E36" s="9">
+      <c r="E36" s="8">
         <v>141.10900000000001</v>
       </c>
       <c r="F36">
@@ -4421,7 +4428,7 @@
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="8">
+      <c r="A37" s="7">
         <v>449</v>
       </c>
       <c r="B37">
@@ -4433,16 +4440,16 @@
       <c r="D37" t="s">
         <v>22</v>
       </c>
-      <c r="E37" s="9">
+      <c r="E37" s="8">
         <v>56453.353000000003</v>
       </c>
-      <c r="H37" s="16">
+      <c r="H37" s="15">
         <f t="shared" ref="H37:H43" si="40">B36/B37</f>
         <v>1.2811380819737366</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="8">
+      <c r="A38" s="7">
         <v>474</v>
       </c>
       <c r="B38">
@@ -4454,7 +4461,7 @@
       <c r="D38" t="s">
         <v>32</v>
       </c>
-      <c r="E38" s="9">
+      <c r="E38" s="8">
         <v>145.678</v>
       </c>
       <c r="F38">
@@ -4471,7 +4478,7 @@
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="8">
+      <c r="A39" s="7">
         <v>474</v>
       </c>
       <c r="B39">
@@ -4483,16 +4490,16 @@
       <c r="D39" t="s">
         <v>29</v>
       </c>
-      <c r="E39" s="9">
+      <c r="E39" s="8">
         <v>66522.074999999997</v>
       </c>
-      <c r="H39" s="16">
+      <c r="H39" s="15">
         <f t="shared" ref="H39:H43" si="42">B38/B39</f>
         <v>1.2493125572868928</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="8">
+      <c r="A40" s="7">
         <v>499</v>
       </c>
       <c r="B40">
@@ -4504,7 +4511,7 @@
       <c r="D40" t="s">
         <v>31</v>
       </c>
-      <c r="E40" s="9">
+      <c r="E40" s="8">
         <v>167.845</v>
       </c>
       <c r="F40">
@@ -4521,7 +4528,7 @@
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="8">
+      <c r="A41" s="7">
         <v>499</v>
       </c>
       <c r="B41">
@@ -4533,16 +4540,16 @@
       <c r="D41" t="s">
         <v>20</v>
       </c>
-      <c r="E41" s="9">
+      <c r="E41" s="8">
         <v>78458.733999999997</v>
       </c>
-      <c r="H41" s="16">
+      <c r="H41" s="15">
         <f t="shared" ref="H41:H43" si="44">B40/B41</f>
         <v>1.3346216436126934</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="8">
+      <c r="A42" s="7">
         <v>524</v>
       </c>
       <c r="B42">
@@ -4554,7 +4561,7 @@
       <c r="D42" t="s">
         <v>33</v>
       </c>
-      <c r="E42" s="9">
+      <c r="E42" s="8">
         <v>185.93100000000001</v>
       </c>
       <c r="F42">
@@ -4571,7 +4578,7 @@
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" s="8">
+      <c r="A43" s="7">
         <v>524</v>
       </c>
       <c r="B43">
@@ -4583,10 +4590,10 @@
       <c r="D43" t="s">
         <v>28</v>
       </c>
-      <c r="E43" s="9">
+      <c r="E43" s="8">
         <v>90990.404999999999</v>
       </c>
-      <c r="H43" s="16">
+      <c r="H43" s="15">
         <f t="shared" ref="H43" si="46">B42/B43</f>
         <v>1.199963937973314</v>
       </c>

</xml_diff>